<commit_message>
Add change to the Ref ID
</commit_message>
<xml_diff>
--- a/tools/ref_audit_ssi_tunisie/Ref_Audit_SSI_TUNISIE.xlsx
+++ b/tools/ref_audit_ssi_tunisie/Ref_Audit_SSI_TUNISIE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imanabshirali/Desktop/stage MAi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imanabshirali/Documents/GitHub/ciso-assistant-community/tools/ref_audit_ssi_tunisie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C85E51B-5F60-9D4E-AA44-4845D0067FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38734713-90D6-6E4C-920F-FFD491C4B308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15520" xr2:uid="{5DB00E7C-FD99-BF41-9C86-24AA98210256}"/>
   </bookViews>
@@ -570,9 +570,6 @@
     <t xml:space="preserve">Référentiel d’Audit de la Sécurité des Systèmes d’Information (ANCS Tunisie) </t>
   </si>
   <si>
-    <t xml:space="preserve">Réferenti-d'Audit-SSI (ANCS Tunisie) </t>
-  </si>
-  <si>
     <t>urn:intuitem:risk:library:referentiel-audit-SSI-ANCS-Tunisie</t>
   </si>
   <si>
@@ -1002,6 +999,9 @@
 mission.
 Lien du Document :
 https://www.ancs.tn/sites/default/files/Referentiel_Audit%203.1.pdf </t>
+  </si>
+  <si>
+    <t>Reférentiel-audit-SSI-ANCS-Tunisie</t>
   </si>
 </sst>
 </file>
@@ -1466,7 +1466,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1481,7 +1481,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -1508,7 +1508,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>176</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1525,7 +1525,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1543,7 +1543,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -1561,7 +1561,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -1570,7 +1570,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>176</v>
+        <v>315</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -1588,7 +1588,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -1653,7 +1653,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F2" s="8"/>
     </row>
@@ -1665,10 +1665,10 @@
         <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="102">
@@ -1693,7 +1693,7 @@
         <v>27</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="51">
@@ -1718,7 +1718,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="51">
@@ -1743,7 +1743,7 @@
         <v>33</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="68">
@@ -1754,7 +1754,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17">
@@ -1768,7 +1768,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="34">
@@ -1793,7 +1793,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="51">
@@ -1818,7 +1818,7 @@
         <v>41</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="51">
@@ -1843,7 +1843,7 @@
         <v>44</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="34">
@@ -1868,7 +1868,7 @@
         <v>76</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="34">
@@ -1890,10 +1890,10 @@
         <v>47</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="51">
@@ -1918,7 +1918,7 @@
         <v>79</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="68">
@@ -1929,7 +1929,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17">
@@ -1943,7 +1943,7 @@
         <v>80</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="68">
@@ -1954,7 +1954,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17">
@@ -1968,7 +1968,7 @@
         <v>81</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="51">
@@ -1979,7 +1979,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="17">
@@ -1993,7 +1993,7 @@
         <v>82</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="68">
@@ -2004,7 +2004,7 @@
         <v>3</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17">
@@ -2018,7 +2018,7 @@
         <v>83</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="68">
@@ -2043,7 +2043,7 @@
         <v>85</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="17">
@@ -2068,7 +2068,7 @@
         <v>87</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="68">
@@ -2093,7 +2093,7 @@
         <v>89</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="68">
@@ -2104,7 +2104,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="34">
@@ -2118,7 +2118,7 @@
         <v>90</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="51">
@@ -2143,7 +2143,7 @@
         <v>92</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="51">
@@ -2168,7 +2168,7 @@
         <v>94</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="51">
@@ -2193,7 +2193,7 @@
         <v>96</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="68">
@@ -2218,7 +2218,7 @@
         <v>98</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="68">
@@ -2243,7 +2243,7 @@
         <v>100</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="85">
@@ -2268,7 +2268,7 @@
         <v>102</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="51">
@@ -2279,7 +2279,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="17">
@@ -2293,7 +2293,7 @@
         <v>103</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="34">
@@ -2318,7 +2318,7 @@
         <v>105</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="51">
@@ -2343,7 +2343,7 @@
         <v>107</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="51">
@@ -2368,7 +2368,7 @@
         <v>109</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="34">
@@ -2393,7 +2393,7 @@
         <v>111</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="51">
@@ -2418,7 +2418,7 @@
         <v>113</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="85">
@@ -2443,7 +2443,7 @@
         <v>115</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="85">
@@ -2468,7 +2468,7 @@
         <v>117</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="85">
@@ -2493,7 +2493,7 @@
         <v>119</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="68">
@@ -2518,7 +2518,7 @@
         <v>124</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="119">
@@ -2543,7 +2543,7 @@
         <v>123</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="51">
@@ -2568,7 +2568,7 @@
         <v>125</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="34">
@@ -2593,7 +2593,7 @@
         <v>127</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F77" s="8"/>
     </row>
@@ -2608,7 +2608,7 @@
         <v>128</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="85">
@@ -2633,7 +2633,7 @@
         <v>149</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="51">
@@ -2658,7 +2658,7 @@
         <v>146</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="102">
@@ -2683,7 +2683,7 @@
         <v>145</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="68">
@@ -2694,7 +2694,7 @@
         <v>3</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="17">
@@ -2708,7 +2708,7 @@
         <v>143</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="85">
@@ -2733,7 +2733,7 @@
         <v>141</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="85">
@@ -2758,7 +2758,7 @@
         <v>140</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="68">
@@ -2769,7 +2769,7 @@
         <v>3</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="17">
@@ -2783,7 +2783,7 @@
         <v>138</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="68">
@@ -2805,10 +2805,10 @@
         <v>7</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F94" s="8"/>
     </row>
@@ -2823,7 +2823,7 @@
         <v>151</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="51">
@@ -2834,7 +2834,7 @@
         <v>3</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="17">
@@ -2848,7 +2848,7 @@
         <v>152</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="34">
@@ -2870,10 +2870,10 @@
         <v>155</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="34">
@@ -2884,7 +2884,7 @@
         <v>3</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="17">
@@ -2895,10 +2895,10 @@
         <v>156</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="34">
@@ -2909,7 +2909,7 @@
         <v>3</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="34">
@@ -2920,10 +2920,10 @@
         <v>157</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="85">
@@ -2934,7 +2934,7 @@
         <v>3</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="17">
@@ -2945,10 +2945,10 @@
         <v>158</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="34">
@@ -2959,7 +2959,7 @@
         <v>3</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="17">
@@ -2970,10 +2970,10 @@
         <v>159</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="68">
@@ -2984,7 +2984,7 @@
         <v>3</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="17">
@@ -2995,10 +2995,10 @@
         <v>160</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="34">
@@ -3009,7 +3009,7 @@
         <v>3</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="17">
@@ -3020,10 +3020,10 @@
         <v>161</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="34">
@@ -3034,7 +3034,7 @@
         <v>3</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="17">
@@ -3045,10 +3045,10 @@
         <v>162</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="68">
@@ -3059,7 +3059,7 @@
         <v>3</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="17">
@@ -3073,7 +3073,7 @@
         <v>172</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="51">
@@ -3098,7 +3098,7 @@
         <v>170</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="51">
@@ -3123,7 +3123,7 @@
         <v>169</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="34">
@@ -3134,7 +3134,7 @@
         <v>3</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="17">
@@ -3148,7 +3148,7 @@
         <v>167</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="85">
@@ -3170,10 +3170,10 @@
         <v>8</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F123" s="8"/>
     </row>
@@ -3182,13 +3182,13 @@
         <v>2</v>
       </c>
       <c r="C124" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="34">
@@ -3199,7 +3199,7 @@
         <v>3</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="17">
@@ -3207,13 +3207,13 @@
         <v>2</v>
       </c>
       <c r="C126" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="34">
@@ -3224,7 +3224,7 @@
         <v>3</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="17">
@@ -3232,13 +3232,13 @@
         <v>2</v>
       </c>
       <c r="C128" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="51">
@@ -3249,7 +3249,7 @@
         <v>3</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="17">
@@ -3257,13 +3257,13 @@
         <v>2</v>
       </c>
       <c r="C130" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="51">
@@ -3274,7 +3274,7 @@
         <v>3</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="17">
@@ -3282,13 +3282,13 @@
         <v>2</v>
       </c>
       <c r="C132" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="51">
@@ -3299,7 +3299,7 @@
         <v>3</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="17">
@@ -3307,13 +3307,13 @@
         <v>2</v>
       </c>
       <c r="C134" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="34">
@@ -3324,7 +3324,7 @@
         <v>3</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="17">
@@ -3332,13 +3332,13 @@
         <v>2</v>
       </c>
       <c r="C136" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="51">
@@ -3349,7 +3349,7 @@
         <v>3</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="17">
@@ -3357,13 +3357,13 @@
         <v>2</v>
       </c>
       <c r="C138" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="68">
@@ -3374,7 +3374,7 @@
         <v>3</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="17">
@@ -3382,13 +3382,13 @@
         <v>2</v>
       </c>
       <c r="C140" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="68">
@@ -3399,7 +3399,7 @@
         <v>3</v>
       </c>
       <c r="E141" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="17">
@@ -3407,13 +3407,13 @@
         <v>2</v>
       </c>
       <c r="C142" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="51">
@@ -3424,7 +3424,7 @@
         <v>3</v>
       </c>
       <c r="E143" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="17">
@@ -3432,13 +3432,13 @@
         <v>2</v>
       </c>
       <c r="C144" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="68">
@@ -3449,7 +3449,7 @@
         <v>3</v>
       </c>
       <c r="E145" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="17">
@@ -3457,13 +3457,13 @@
         <v>2</v>
       </c>
       <c r="C146" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E146" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="68">
@@ -3474,7 +3474,7 @@
         <v>3</v>
       </c>
       <c r="E147" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="17">
@@ -3482,13 +3482,13 @@
         <v>2</v>
       </c>
       <c r="C148" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="51">
@@ -3499,7 +3499,7 @@
         <v>3</v>
       </c>
       <c r="E149" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="17">
@@ -3507,13 +3507,13 @@
         <v>2</v>
       </c>
       <c r="C150" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="51">
@@ -3524,7 +3524,7 @@
         <v>3</v>
       </c>
       <c r="E151" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="17">
@@ -3532,13 +3532,13 @@
         <v>2</v>
       </c>
       <c r="C152" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E152" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="51">
@@ -3549,7 +3549,7 @@
         <v>3</v>
       </c>
       <c r="E153" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="17">
@@ -3557,13 +3557,13 @@
         <v>2</v>
       </c>
       <c r="C154" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E154" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="68">
@@ -3574,7 +3574,7 @@
         <v>3</v>
       </c>
       <c r="E155" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="17">
@@ -3582,13 +3582,13 @@
         <v>2</v>
       </c>
       <c r="C156" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E156" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="51">
@@ -3599,7 +3599,7 @@
         <v>3</v>
       </c>
       <c r="E157" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="17">
@@ -3607,13 +3607,13 @@
         <v>2</v>
       </c>
       <c r="C158" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E158" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="51">
@@ -3624,7 +3624,7 @@
         <v>3</v>
       </c>
       <c r="E159" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="17">
@@ -3632,13 +3632,13 @@
         <v>2</v>
       </c>
       <c r="C160" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E160" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="51">
@@ -3649,7 +3649,7 @@
         <v>3</v>
       </c>
       <c r="E161" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="17">
@@ -3657,13 +3657,13 @@
         <v>2</v>
       </c>
       <c r="C162" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E162" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="51">
@@ -3674,7 +3674,7 @@
         <v>3</v>
       </c>
       <c r="E163" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="17">
@@ -3682,13 +3682,13 @@
         <v>2</v>
       </c>
       <c r="C164" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="51">
@@ -3699,7 +3699,7 @@
         <v>3</v>
       </c>
       <c r="E165" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="17">
@@ -3707,13 +3707,13 @@
         <v>2</v>
       </c>
       <c r="C166" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E166" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="51">
@@ -3724,7 +3724,7 @@
         <v>3</v>
       </c>
       <c r="E167" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="17">
@@ -3732,13 +3732,13 @@
         <v>2</v>
       </c>
       <c r="C168" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E168" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="34">
@@ -3749,7 +3749,7 @@
         <v>3</v>
       </c>
       <c r="E169" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="17">
@@ -3757,13 +3757,13 @@
         <v>2</v>
       </c>
       <c r="C170" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E170" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="51">
@@ -3774,7 +3774,7 @@
         <v>3</v>
       </c>
       <c r="E171" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="17">
@@ -3782,13 +3782,13 @@
         <v>2</v>
       </c>
       <c r="C172" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E172" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="34">
@@ -3799,7 +3799,7 @@
         <v>3</v>
       </c>
       <c r="E173" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="17">
@@ -3807,13 +3807,13 @@
         <v>2</v>
       </c>
       <c r="C174" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D174" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E174" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="51">
@@ -3824,7 +3824,7 @@
         <v>3</v>
       </c>
       <c r="E175" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="34">
@@ -3832,13 +3832,13 @@
         <v>2</v>
       </c>
       <c r="C176" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D176" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E176" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="51">
@@ -3849,7 +3849,7 @@
         <v>3</v>
       </c>
       <c r="E177" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="17">
@@ -3857,13 +3857,13 @@
         <v>2</v>
       </c>
       <c r="C178" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D178" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E178" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="34">
@@ -3874,7 +3874,7 @@
         <v>3</v>
       </c>
       <c r="E179" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="17">
@@ -3882,13 +3882,13 @@
         <v>2</v>
       </c>
       <c r="C180" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D180" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E180" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="34">
@@ -3899,7 +3899,7 @@
         <v>3</v>
       </c>
       <c r="E181" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="17">
@@ -3907,13 +3907,13 @@
         <v>2</v>
       </c>
       <c r="C182" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D182" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E182" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="34">
@@ -3924,7 +3924,7 @@
         <v>3</v>
       </c>
       <c r="E183" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="34">
@@ -3932,13 +3932,13 @@
         <v>2</v>
       </c>
       <c r="C184" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D184" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E184" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="68">
@@ -3949,7 +3949,7 @@
         <v>3</v>
       </c>
       <c r="E185" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="17">
@@ -3957,13 +3957,13 @@
         <v>2</v>
       </c>
       <c r="C186" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D186" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E186" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="51">
@@ -3974,7 +3974,7 @@
         <v>3</v>
       </c>
       <c r="E187" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="17">
@@ -3982,13 +3982,13 @@
         <v>2</v>
       </c>
       <c r="C188" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D188" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E188" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="34">
@@ -3999,7 +3999,7 @@
         <v>3</v>
       </c>
       <c r="E189" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="34">
@@ -4007,13 +4007,13 @@
         <v>2</v>
       </c>
       <c r="C190" t="s">
+        <v>227</v>
+      </c>
+      <c r="D190" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="D190" s="5" t="s">
-        <v>229</v>
-      </c>
       <c r="E190" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="68">
@@ -4024,7 +4024,7 @@
         <v>3</v>
       </c>
       <c r="E191" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>